<commit_message>
cost calculation & correct trading hours: HE, LE, GF
</commit_message>
<xml_diff>
--- a/custom/gscbt/gscbt/data/iqfeed_data.xlsx
+++ b/custom/gscbt/gscbt/data/iqfeed_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBISP\anurag\.envs\gscap\Lib\site-packages\gscbt\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBISP\anurag\gsc\gscap\custom\gscbt\gscbt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F6778-8468-4156-AF37-00FA98338E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BE194C-65B6-4DBB-AF3E-1CB73B35C9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OHLCV_data" sheetId="1" r:id="rId1"/>
@@ -44,8 +44,28 @@
 </workbook>
 </file>
 
+<file path=xl/python.xml><?xml version="1.0" encoding="utf-8"?>
+<python xmlns="http://schemas.microsoft.com/office/spreadsheetml/2023/python">
+  <environmentDefinition id="{882DD1B0-6546-4DFA-8A08-902A380B44EA}">
+    <initialization>
+      <code xml:space="preserve">import numpy as np
+import pandas as pd
+import matplotlib.pyplot as plt
+import seaborn as sns
+import statsmodels as sm
+import excel
+import warnings
+warnings.simplefilter('ignore')
+excel.set_xl_scalar_conversion(excel.convert_to_scalar)
+excel.set_xl_array_conversion(excel.convert_to_dataframe)
+</code>
+    </initialization>
+  </environmentDefinition>
+</python>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3748" uniqueCount="3170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3752" uniqueCount="3174">
   <si>
     <t>IQ FEED SYMBOL MAPPING</t>
   </si>
@@ -9555,6 +9575,18 @@
   </si>
   <si>
     <t>Mini Future</t>
+  </si>
+  <si>
+    <t>Trading Hours</t>
+  </si>
+  <si>
+    <t>Currency Tick Value</t>
+  </si>
+  <si>
+    <t>Cost in Ticks</t>
+  </si>
+  <si>
+    <t>Commission Cost</t>
   </si>
 </sst>
 </file>
@@ -9565,7 +9597,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9716,12 +9748,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
@@ -9777,34 +9803,29 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF212529"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF212529"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="41">
@@ -10036,7 +10057,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -10194,6 +10215,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -10241,59 +10282,59 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="34" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="34" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -10301,95 +10342,98 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="39" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="18" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="40" borderId="10" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="39" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="26" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="28" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="26" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="31" fillId="40" borderId="10" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="40" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="40" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="26" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -10748,2365 +10792,3137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" style="49" customWidth="1"/>
-    <col min="2" max="2" width="13" style="49" customWidth="1"/>
-    <col min="3" max="3" width="14" style="49" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="49" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="66" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="49" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="49" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="49" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="52" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="49" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="49" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="49"/>
+    <col min="1" max="1" width="48.7109375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="13" style="52" customWidth="1"/>
+    <col min="3" max="3" width="14" style="52" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="78" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="52" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="79" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="52" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="52" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="52" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" style="78" customWidth="1"/>
+    <col min="12" max="13" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="52" customWidth="1"/>
+    <col min="15" max="16" width="12.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-    </row>
-    <row r="2" spans="1:12" s="50" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+    </row>
+    <row r="2" spans="1:16" s="56" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="53" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="M2" s="53" t="s">
+        <v>3171</v>
+      </c>
+      <c r="N2" s="53" t="s">
+        <v>3172</v>
+      </c>
+      <c r="O2" s="53" t="s">
+        <v>3173</v>
+      </c>
+      <c r="P2" s="53" t="s">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="60">
         <v>34702</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="61">
         <v>1000</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58">
         <v>1000</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="69" t="s">
+      <c r="L3" s="58" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="M3" s="58">
+        <v>10</v>
+      </c>
+      <c r="N3" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="62">
+        <v>1.07</v>
+      </c>
+      <c r="P3" s="58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="55">
+      <c r="E4" s="66">
         <v>34702</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="67">
         <v>25000</v>
       </c>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53">
+      <c r="I4" s="64"/>
+      <c r="J4" s="64">
         <v>25000</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="53" t="s">
+      <c r="L4" s="64" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
+      <c r="M4" s="58">
+        <v>12.5</v>
+      </c>
+      <c r="N4" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O4" s="62">
+        <v>1.17</v>
+      </c>
+      <c r="P4" s="58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="71">
         <v>34702</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="G5" s="65">
+      <c r="G5" s="72">
         <v>42000</v>
       </c>
-      <c r="H5" s="72" t="s">
+      <c r="H5" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72">
+      <c r="I5" s="62"/>
+      <c r="J5" s="62">
         <v>42000</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="62" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="M5" s="58">
+        <v>4.2</v>
+      </c>
+      <c r="N5" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="62">
+        <v>1.07</v>
+      </c>
+      <c r="P5" s="58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="72" t="s">
+      <c r="D6" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="66">
         <v>34702</v>
       </c>
-      <c r="F6" s="72" t="s">
+      <c r="F6" s="62" t="s">
         <v>3163</v>
       </c>
-      <c r="G6" s="64">
+      <c r="G6" s="67">
         <v>50</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="H6" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72">
+      <c r="I6" s="62"/>
+      <c r="J6" s="62">
         <v>50</v>
       </c>
-      <c r="K6" s="73" t="s">
+      <c r="K6" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="72" t="s">
+      <c r="L6" s="62" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="M6" s="58">
+        <v>12.5</v>
+      </c>
+      <c r="N6" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O6" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P6" s="62">
+        <v>17.58333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="74">
+      <c r="E7" s="71">
         <v>34702</v>
       </c>
-      <c r="F7" s="72" t="s">
+      <c r="F7" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="G7" s="65">
+      <c r="G7" s="72">
         <v>10000</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72">
+      <c r="I7" s="62"/>
+      <c r="J7" s="62">
         <v>10000</v>
       </c>
-      <c r="K7" s="73" t="s">
+      <c r="K7" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="72" t="s">
+      <c r="L7" s="62" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+      <c r="M7" s="62">
+        <v>10</v>
+      </c>
+      <c r="N7" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="62">
+        <v>1</v>
+      </c>
+      <c r="P7" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="71">
         <v>34702</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="G8" s="65">
+      <c r="G8" s="72">
         <v>42000</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72">
+      <c r="I8" s="62"/>
+      <c r="J8" s="62">
         <v>42000</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="72" t="s">
+      <c r="L8" s="62" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="M8" s="58">
+        <v>4.2</v>
+      </c>
+      <c r="N8" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O8" s="62">
+        <v>1.07</v>
+      </c>
+      <c r="P8" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="74">
+      <c r="E9" s="71">
         <v>41439</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="72">
         <v>1000</v>
       </c>
-      <c r="H9" s="72" t="s">
+      <c r="H9" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72">
+      <c r="I9" s="62"/>
+      <c r="J9" s="62">
         <v>1000</v>
       </c>
-      <c r="K9" s="73" t="s">
+      <c r="K9" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="72" t="s">
+      <c r="L9" s="62" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
+      <c r="M9" s="62">
+        <v>5</v>
+      </c>
+      <c r="N9" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O9" s="62">
+        <v>1.17</v>
+      </c>
+      <c r="P9" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="74">
+      <c r="E10" s="71">
         <v>34702</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="62" t="s">
         <v>3163</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="72">
         <v>50</v>
       </c>
-      <c r="H10" s="72" t="s">
+      <c r="H10" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72">
+      <c r="I10" s="62"/>
+      <c r="J10" s="62">
         <v>50</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="72" t="s">
+      <c r="L10" s="62" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
+      <c r="M10" s="58">
+        <v>12.5</v>
+      </c>
+      <c r="N10" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O10" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P10" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="74">
+      <c r="E11" s="71">
         <v>34702</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="62" t="s">
         <v>3163</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="72">
         <v>600</v>
       </c>
-      <c r="H11" s="72" t="s">
+      <c r="H11" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72">
+      <c r="I11" s="62"/>
+      <c r="J11" s="62">
         <v>600</v>
       </c>
-      <c r="K11" s="73" t="s">
+      <c r="K11" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="L11" s="53" t="s">
+      <c r="L11" s="64" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="M11" s="62">
+        <v>6</v>
+      </c>
+      <c r="N11" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O11" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P11" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="74">
+      <c r="E12" s="71">
         <v>34702</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="62" t="s">
         <v>3163</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="72">
         <v>100</v>
       </c>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72">
+      <c r="I12" s="62"/>
+      <c r="J12" s="62">
         <v>100</v>
       </c>
-      <c r="K12" s="73" t="s">
+      <c r="K12" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="72" t="s">
+      <c r="L12" s="62" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="M12" s="62">
+        <v>10</v>
+      </c>
+      <c r="N12" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P12" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="74">
+      <c r="E13" s="71">
         <v>34702</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="62" t="s">
         <v>3163</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="72">
         <v>50</v>
       </c>
-      <c r="H13" s="72" t="s">
+      <c r="H13" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72">
+      <c r="I13" s="62"/>
+      <c r="J13" s="62">
         <v>50</v>
       </c>
-      <c r="K13" s="73" t="s">
+      <c r="K13" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="72" t="s">
+      <c r="L13" s="62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="M13" s="62">
+        <v>12.5</v>
+      </c>
+      <c r="N13" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O13" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P13" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="74">
+      <c r="E14" s="71">
         <v>34702</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="62" t="s">
         <v>3163</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="72">
         <v>50</v>
       </c>
-      <c r="H14" s="72" t="s">
+      <c r="H14" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72">
+      <c r="I14" s="62"/>
+      <c r="J14" s="62">
         <v>50</v>
       </c>
-      <c r="K14" s="73" t="s">
+      <c r="K14" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="72" t="s">
+      <c r="L14" s="62" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="61" t="s">
+      <c r="M14" s="62">
+        <v>12.5</v>
+      </c>
+      <c r="N14" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O14" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P14" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="74">
+      <c r="E15" s="71">
         <v>34709</v>
       </c>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="72">
         <v>100</v>
       </c>
-      <c r="H15" s="72" t="s">
+      <c r="H15" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72">
+      <c r="I15" s="62"/>
+      <c r="J15" s="62">
         <v>100</v>
       </c>
-      <c r="K15" s="73" t="s">
+      <c r="K15" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="72" t="s">
+      <c r="L15" s="62" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="M15" s="62">
+        <v>50</v>
+      </c>
+      <c r="N15" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O15" s="62">
+        <v>1</v>
+      </c>
+      <c r="P15" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="74">
+      <c r="E16" s="71">
         <v>34702</v>
       </c>
-      <c r="F16" s="72" t="s">
+      <c r="F16" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="G16" s="65">
+      <c r="G16" s="72">
         <v>50</v>
       </c>
-      <c r="H16" s="72" t="s">
+      <c r="H16" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72">
+      <c r="I16" s="62"/>
+      <c r="J16" s="62">
         <v>50</v>
       </c>
-      <c r="K16" s="73" t="s">
+      <c r="K16" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="72" t="s">
+      <c r="L16" s="62" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="M16" s="62">
+        <v>5</v>
+      </c>
+      <c r="N16" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O16" s="62">
+        <v>1</v>
+      </c>
+      <c r="P16" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="72" t="s">
+      <c r="D17" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="74">
+      <c r="E17" s="71">
         <v>34702</v>
       </c>
-      <c r="F17" s="72" t="s">
+      <c r="F17" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="G17" s="65">
+      <c r="G17" s="72">
         <v>5000</v>
       </c>
-      <c r="H17" s="72" t="s">
+      <c r="H17" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72">
+      <c r="I17" s="62"/>
+      <c r="J17" s="62">
         <v>5000</v>
       </c>
-      <c r="K17" s="73" t="s">
+      <c r="K17" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="72" t="s">
+      <c r="L17" s="62" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
+      <c r="M17" s="62">
+        <v>25</v>
+      </c>
+      <c r="N17" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O17" s="62">
+        <v>1.17</v>
+      </c>
+      <c r="P17" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="74">
+      <c r="E18" s="71">
         <v>34702</v>
       </c>
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="G18" s="65">
+      <c r="G18" s="72">
         <v>400</v>
       </c>
-      <c r="H18" s="72" t="s">
+      <c r="H18" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72">
+      <c r="I18" s="62"/>
+      <c r="J18" s="62">
         <v>400</v>
       </c>
-      <c r="K18" s="73" t="s">
+      <c r="K18" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="L18" s="72" t="s">
+      <c r="L18" s="62" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+      <c r="M18" s="62">
+        <v>10</v>
+      </c>
+      <c r="N18" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O18" s="62">
+        <v>1.06</v>
+      </c>
+      <c r="P18" s="62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="74">
+      <c r="E19" s="71">
         <v>36984</v>
       </c>
-      <c r="F19" s="72" t="s">
+      <c r="F19" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="G19" s="65">
+      <c r="G19" s="72">
         <v>500</v>
       </c>
-      <c r="H19" s="72" t="s">
+      <c r="H19" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72">
+      <c r="I19" s="62"/>
+      <c r="J19" s="62">
         <v>500</v>
       </c>
-      <c r="K19" s="73" t="s">
+      <c r="K19" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="72" t="s">
+      <c r="L19" s="62" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="M19" s="62">
+        <v>12.5</v>
+      </c>
+      <c r="N19" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O19" s="62">
+        <v>1.06</v>
+      </c>
+      <c r="P19" s="62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="74">
+      <c r="E20" s="71">
         <v>34702</v>
       </c>
-      <c r="F20" s="72" t="s">
+      <c r="F20" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="G20" s="65">
+      <c r="G20" s="72">
         <v>400</v>
       </c>
-      <c r="H20" s="72" t="s">
+      <c r="H20" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72">
+      <c r="I20" s="62"/>
+      <c r="J20" s="62">
         <v>400</v>
       </c>
-      <c r="K20" s="73" t="s">
+      <c r="K20" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="L20" s="72" t="s">
+      <c r="L20" s="62" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
+      <c r="M20" s="62">
+        <v>10</v>
+      </c>
+      <c r="N20" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O20" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P20" s="62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="74">
+      <c r="E21" s="71">
         <v>34702</v>
       </c>
-      <c r="F21" s="72" t="s">
+      <c r="F21" s="62" t="s">
         <v>3164</v>
       </c>
-      <c r="G21" s="65">
+      <c r="G21" s="72">
         <v>1000</v>
       </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72">
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62">
         <v>1000</v>
       </c>
-      <c r="K21" s="73" t="s">
+      <c r="K21" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L21" s="72" t="s">
+      <c r="L21" s="62" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="M21" s="62">
+        <v>15.625</v>
+      </c>
+      <c r="N21" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O21" s="62">
+        <v>1</v>
+      </c>
+      <c r="P21" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="74">
+      <c r="E22" s="71">
         <v>34702</v>
       </c>
-      <c r="F22" s="72" t="s">
+      <c r="F22" s="62" t="s">
         <v>3164</v>
       </c>
-      <c r="G22" s="65">
+      <c r="G22" s="72">
         <v>1000</v>
       </c>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="65">
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="72">
         <v>1000</v>
       </c>
-      <c r="K22" s="73" t="s">
+      <c r="K22" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L22" s="72" t="s">
+      <c r="L22" s="62" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="M22" s="62">
+        <v>31.25</v>
+      </c>
+      <c r="N22" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O22" s="62">
+        <v>1</v>
+      </c>
+      <c r="P22" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="74">
+      <c r="E23" s="71">
         <v>35116</v>
       </c>
-      <c r="F23" s="72" t="s">
+      <c r="F23" s="62" t="s">
         <v>3164</v>
       </c>
-      <c r="G23" s="65">
+      <c r="G23" s="72">
         <v>4167</v>
       </c>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="65">
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="72">
         <v>4167</v>
       </c>
-      <c r="K23" s="73" t="s">
+      <c r="K23" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="72" t="s">
+      <c r="L23" s="62" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="M23" s="62">
+        <v>20.835000000000001</v>
+      </c>
+      <c r="N23" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O23" s="62">
+        <v>1</v>
+      </c>
+      <c r="P23" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="72" t="s">
+      <c r="D24" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="74">
+      <c r="E24" s="71">
         <v>43224</v>
       </c>
-      <c r="F24" s="72" t="s">
+      <c r="F24" s="62" t="s">
         <v>3164</v>
       </c>
-      <c r="G24" s="65">
+      <c r="G24" s="72">
         <v>4167</v>
       </c>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72">
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62">
         <v>4167</v>
       </c>
-      <c r="K24" s="73" t="s">
+      <c r="K24" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L24" s="72" t="s">
+      <c r="L24" s="62" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="M24" s="62">
+        <v>10.4175</v>
+      </c>
+      <c r="N24" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O24" s="62">
+        <v>1</v>
+      </c>
+      <c r="P24" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="69" t="s">
         <v>162</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="D25" s="72" t="s">
+      <c r="D25" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="74">
+      <c r="E25" s="71">
         <v>35682</v>
       </c>
-      <c r="F25" s="72" t="s">
+      <c r="F25" s="62" t="s">
         <v>552</v>
       </c>
-      <c r="G25" s="65">
+      <c r="G25" s="72">
         <v>50</v>
       </c>
-      <c r="H25" s="72" t="s">
+      <c r="H25" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72">
+      <c r="I25" s="62"/>
+      <c r="J25" s="62">
         <v>50</v>
       </c>
-      <c r="K25" s="73" t="s">
+      <c r="K25" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L25" s="72" t="s">
+      <c r="L25" s="62" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+      <c r="M25" s="62">
+        <v>12.5</v>
+      </c>
+      <c r="N25" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O25" s="62">
+        <v>0.92</v>
+      </c>
+      <c r="P25" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
         <v>172</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="75" t="s">
         <v>173</v>
       </c>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="76" t="s">
+      <c r="D26" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="74">
+      <c r="E26" s="71">
         <v>43224</v>
       </c>
-      <c r="F26" s="72" t="s">
+      <c r="F26" s="62" t="s">
         <v>3164</v>
       </c>
-      <c r="G26" s="65">
+      <c r="G26" s="72">
         <v>2500</v>
       </c>
-      <c r="H26" s="72" t="s">
+      <c r="H26" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72">
+      <c r="I26" s="62"/>
+      <c r="J26" s="62">
         <v>2500</v>
       </c>
-      <c r="K26" s="73" t="s">
+      <c r="K26" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L26" s="72" t="s">
+      <c r="L26" s="62" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
+      <c r="M26" s="62">
+        <v>6.25</v>
+      </c>
+      <c r="N26" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O26" s="62">
+        <v>0.67</v>
+      </c>
+      <c r="P26" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="69" t="s">
         <v>185</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="73" t="s">
+      <c r="C27" s="70" t="s">
         <v>187</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="74">
+      <c r="E27" s="71">
         <v>34702</v>
       </c>
-      <c r="F27" s="72" t="s">
+      <c r="F27" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="G27" s="65">
+      <c r="G27" s="72">
         <v>100</v>
       </c>
-      <c r="H27" s="72" t="s">
+      <c r="H27" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="72"/>
-      <c r="J27" s="72">
+      <c r="I27" s="62"/>
+      <c r="J27" s="62">
         <v>100</v>
       </c>
-      <c r="K27" s="73" t="s">
+      <c r="K27" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L27" s="72" t="s">
+      <c r="L27" s="62" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+      <c r="M27" s="62">
+        <v>10</v>
+      </c>
+      <c r="N27" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O27" s="62">
+        <v>1.17</v>
+      </c>
+      <c r="P27" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="69" t="s">
         <v>189</v>
       </c>
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="70" t="s">
         <v>191</v>
       </c>
-      <c r="D28" s="72" t="s">
+      <c r="D28" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="74">
+      <c r="E28" s="71">
         <v>36332</v>
       </c>
-      <c r="F28" s="72" t="s">
+      <c r="F28" s="62" t="s">
         <v>552</v>
       </c>
-      <c r="G28" s="65">
+      <c r="G28" s="72">
         <v>20</v>
       </c>
-      <c r="H28" s="72" t="s">
+      <c r="H28" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72">
+      <c r="I28" s="62"/>
+      <c r="J28" s="62">
         <v>20</v>
       </c>
-      <c r="K28" s="73" t="s">
+      <c r="K28" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L28" s="72" t="s">
+      <c r="L28" s="62" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="61" t="s">
+      <c r="M28" s="62">
+        <v>5</v>
+      </c>
+      <c r="N28" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O28" s="62">
+        <v>1</v>
+      </c>
+      <c r="P28" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="62" t="s">
         <v>199</v>
       </c>
-      <c r="C29" s="73" t="s">
+      <c r="C29" s="70" t="s">
         <v>200</v>
       </c>
-      <c r="D29" s="72" t="s">
+      <c r="D29" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="74">
+      <c r="E29" s="71">
         <v>40763</v>
       </c>
-      <c r="F29" s="72" t="s">
+      <c r="F29" s="62" t="s">
         <v>3165</v>
       </c>
-      <c r="G29" s="65">
+      <c r="G29" s="72">
         <v>100</v>
       </c>
-      <c r="H29" s="72" t="s">
+      <c r="H29" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72">
+      <c r="I29" s="62"/>
+      <c r="J29" s="62">
         <v>100</v>
       </c>
-      <c r="K29" s="73" t="s">
+      <c r="K29" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L29" s="72" t="s">
+      <c r="L29" s="62" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="61" t="s">
+      <c r="M29" s="62">
+        <v>1</v>
+      </c>
+      <c r="N29" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O29" s="62">
+        <v>1</v>
+      </c>
+      <c r="P29" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="69" t="s">
         <v>202</v>
       </c>
-      <c r="B30" s="72" t="s">
+      <c r="B30" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="C30" s="73" t="s">
+      <c r="C30" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="D30" s="72" t="s">
+      <c r="D30" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="74">
+      <c r="E30" s="71">
         <v>34702</v>
       </c>
-      <c r="F30" s="72" t="s">
+      <c r="F30" s="62" t="s">
         <v>3165</v>
       </c>
-      <c r="G30" s="65">
+      <c r="G30" s="72">
         <v>10</v>
       </c>
-      <c r="H30" s="72" t="s">
+      <c r="H30" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72">
+      <c r="I30" s="62"/>
+      <c r="J30" s="62">
         <v>10</v>
       </c>
-      <c r="K30" s="73" t="s">
+      <c r="K30" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="L30" s="72" t="s">
+      <c r="L30" s="62" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="61" t="s">
+      <c r="M30" s="62">
+        <v>1</v>
+      </c>
+      <c r="N30" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O30" s="62">
+        <v>0.77</v>
+      </c>
+      <c r="P30" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="62" t="s">
         <v>207</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C31" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="D31" s="72" t="s">
+      <c r="D31" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="74">
+      <c r="E31" s="71">
         <v>34702</v>
       </c>
-      <c r="F31" s="72" t="s">
+      <c r="F31" s="62" t="s">
         <v>3165</v>
       </c>
-      <c r="G31" s="65">
+      <c r="G31" s="72">
         <v>2500</v>
       </c>
-      <c r="H31" s="72" t="s">
+      <c r="H31" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="72"/>
-      <c r="J31" s="72">
+      <c r="I31" s="62"/>
+      <c r="J31" s="62">
         <v>2500</v>
       </c>
-      <c r="K31" s="73" t="s">
+      <c r="K31" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="72" t="s">
+      <c r="L31" s="62" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="61" t="s">
+      <c r="M31" s="62">
+        <v>1.25</v>
+      </c>
+      <c r="N31" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O31" s="62">
+        <v>0.77</v>
+      </c>
+      <c r="P31" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="69" t="s">
         <v>210</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="C32" s="75" t="s">
+      <c r="C32" s="74" t="s">
         <v>212</v>
       </c>
-      <c r="D32" s="72" t="s">
+      <c r="D32" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="74">
+      <c r="E32" s="71">
         <v>36332</v>
       </c>
-      <c r="F32" s="72" t="s">
+      <c r="F32" s="62" t="s">
         <v>3165</v>
       </c>
-      <c r="G32" s="65">
+      <c r="G32" s="72">
         <v>2</v>
       </c>
-      <c r="H32" s="72" t="s">
+      <c r="H32" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72">
+      <c r="I32" s="62"/>
+      <c r="J32" s="62">
         <v>2</v>
       </c>
-      <c r="K32" s="73" t="s">
+      <c r="K32" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L32" s="72" t="s">
+      <c r="L32" s="62" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="61" t="s">
+      <c r="M32" s="62">
+        <v>5</v>
+      </c>
+      <c r="N32" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O32" s="62">
+        <v>0.35</v>
+      </c>
+      <c r="P32" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="B33" s="72" t="s">
+      <c r="B33" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="C33" s="73" t="s">
+      <c r="C33" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="D33" s="72" t="s">
+      <c r="D33" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="74">
+      <c r="E33" s="71">
         <v>35682</v>
       </c>
-      <c r="F33" s="72" t="s">
+      <c r="F33" s="62" t="s">
         <v>3165</v>
       </c>
-      <c r="G33" s="65">
+      <c r="G33" s="72">
         <v>5</v>
       </c>
-      <c r="H33" s="72" t="s">
+      <c r="H33" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72">
+      <c r="I33" s="62"/>
+      <c r="J33" s="62">
         <v>5</v>
       </c>
-      <c r="K33" s="73" t="s">
+      <c r="K33" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L33" s="72" t="s">
+      <c r="L33" s="62" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+      <c r="M33" s="62">
+        <v>1.25</v>
+      </c>
+      <c r="N33" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O33" s="62">
+        <v>0.35</v>
+      </c>
+      <c r="P33" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="69" t="s">
         <v>223</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="D34" s="72" t="s">
+      <c r="D34" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="74">
+      <c r="E34" s="71">
         <v>38327</v>
       </c>
-      <c r="F34" s="72" t="s">
+      <c r="F34" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="G34" s="65">
+      <c r="G34" s="72">
         <v>2500</v>
       </c>
-      <c r="H34" s="72" t="s">
+      <c r="H34" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72">
+      <c r="I34" s="62"/>
+      <c r="J34" s="62">
         <v>2500</v>
       </c>
-      <c r="K34" s="73" t="s">
+      <c r="K34" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="72" t="s">
+      <c r="L34" s="62" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="61" t="s">
+      <c r="M34" s="62"/>
+      <c r="N34" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O34" s="62">
+        <v>1</v>
+      </c>
+      <c r="P34" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="62" t="s">
         <v>240</v>
       </c>
-      <c r="C35" s="76" t="s">
+      <c r="C35" s="75" t="s">
         <v>241</v>
       </c>
-      <c r="D35" s="73" t="s">
+      <c r="D35" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="74">
+      <c r="E35" s="71">
         <v>37236</v>
       </c>
-      <c r="F35" s="72" t="s">
+      <c r="F35" s="62" t="s">
         <v>552</v>
       </c>
-      <c r="G35" s="65">
+      <c r="G35" s="72">
         <v>50</v>
       </c>
-      <c r="H35" s="72" t="s">
+      <c r="H35" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I35" s="72"/>
-      <c r="J35" s="65">
+      <c r="I35" s="62"/>
+      <c r="J35" s="72">
         <v>50</v>
       </c>
-      <c r="K35" s="73" t="s">
+      <c r="K35" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L35" s="72" t="s">
+      <c r="L35" s="62" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="61" t="s">
+      <c r="M35" s="62">
+        <v>5</v>
+      </c>
+      <c r="N35" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O35" s="62">
+        <v>0.92</v>
+      </c>
+      <c r="P35" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="69" t="s">
         <v>243</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="C36" s="76" t="s">
+      <c r="C36" s="75" t="s">
         <v>245</v>
       </c>
-      <c r="D36" s="73" t="s">
+      <c r="D36" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="74">
+      <c r="E36" s="71">
         <v>37351</v>
       </c>
-      <c r="F36" s="72" t="s">
+      <c r="F36" s="62" t="s">
         <v>552</v>
       </c>
-      <c r="G36" s="65">
+      <c r="G36" s="72">
         <v>5</v>
       </c>
-      <c r="H36" s="72" t="s">
+      <c r="H36" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="72"/>
-      <c r="J36" s="65">
+      <c r="I36" s="62"/>
+      <c r="J36" s="72">
         <v>5</v>
       </c>
-      <c r="K36" s="73" t="s">
+      <c r="K36" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L36" s="72" t="s">
+      <c r="L36" s="62" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="61" t="s">
+      <c r="M36" s="62">
+        <v>5</v>
+      </c>
+      <c r="N36" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O36" s="62">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P36" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="69" t="s">
         <v>247</v>
       </c>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="62" t="s">
         <v>3160</v>
       </c>
-      <c r="C37" s="76" t="s">
+      <c r="C37" s="75" t="s">
         <v>249</v>
       </c>
-      <c r="D37" s="73" t="s">
+      <c r="D37" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="74">
+      <c r="E37" s="71">
         <v>34919</v>
       </c>
-      <c r="F37" s="72" t="s">
+      <c r="F37" s="62" t="s">
         <v>3166</v>
       </c>
-      <c r="G37" s="65"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="73" t="s">
+      <c r="G37" s="72"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L37" s="72"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="61" t="s">
+      <c r="L37" s="62"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O37" s="62">
+        <v>1</v>
+      </c>
+      <c r="P37" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="69" t="s">
         <v>250</v>
       </c>
-      <c r="B38" s="72" t="s">
+      <c r="B38" s="62" t="s">
         <v>3161</v>
       </c>
-      <c r="C38" s="76" t="s">
+      <c r="C38" s="75" t="s">
         <v>252</v>
       </c>
-      <c r="D38" s="73" t="s">
+      <c r="D38" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="74">
+      <c r="E38" s="71">
         <v>34905</v>
       </c>
-      <c r="F38" s="72" t="s">
+      <c r="F38" s="62" t="s">
         <v>3166</v>
       </c>
-      <c r="G38" s="65"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="73" t="s">
+      <c r="G38" s="72"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="72"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="61" t="s">
+      <c r="L38" s="62"/>
+      <c r="M38" s="62"/>
+      <c r="N38" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O38" s="62">
+        <v>1</v>
+      </c>
+      <c r="P38" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="69" t="s">
         <v>257</v>
       </c>
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="C39" s="76" t="s">
+      <c r="C39" s="75" t="s">
         <v>259</v>
       </c>
-      <c r="D39" s="73" t="s">
+      <c r="D39" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="74">
+      <c r="E39" s="71">
         <v>44778</v>
       </c>
-      <c r="F39" s="72" t="s">
+      <c r="F39" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="G39" s="65"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="73" t="s">
+      <c r="G39" s="72"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="L39" s="72" t="s">
+      <c r="L39" s="62" t="s">
         <v>3135</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
+      <c r="M39" s="62"/>
+      <c r="N39" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O39" s="62">
+        <v>1</v>
+      </c>
+      <c r="P39" s="62">
+        <v>6.0833329999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="69" t="s">
         <v>263</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="62" t="s">
         <v>264</v>
       </c>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="75" t="s">
         <v>265</v>
       </c>
-      <c r="D40" s="73" t="s">
+      <c r="D40" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="74">
+      <c r="E40" s="71">
         <v>35219</v>
       </c>
-      <c r="F40" s="72" t="s">
+      <c r="F40" s="62" t="s">
         <v>3164</v>
       </c>
-      <c r="G40" s="65">
+      <c r="G40" s="72">
         <v>2000</v>
       </c>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="65">
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="72">
         <v>2000</v>
       </c>
-      <c r="K40" s="73" t="s">
+      <c r="K40" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L40" s="72" t="s">
+      <c r="L40" s="62" t="s">
         <v>3137</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="61" t="s">
+      <c r="M40" s="62"/>
+      <c r="N40" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O40" s="62">
+        <v>1</v>
+      </c>
+      <c r="P40" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="69" t="s">
         <v>266</v>
       </c>
-      <c r="B41" s="72" t="s">
+      <c r="B41" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="D41" s="73" t="s">
+      <c r="D41" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="74">
+      <c r="E41" s="71">
         <v>34905</v>
       </c>
-      <c r="F41" s="72" t="s">
+      <c r="F41" s="62" t="s">
         <v>3164</v>
       </c>
-      <c r="G41" s="65">
+      <c r="G41" s="72">
         <v>1000</v>
       </c>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="65">
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="72">
         <v>1000</v>
       </c>
-      <c r="K41" s="73" t="s">
+      <c r="K41" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L41" s="72" t="s">
+      <c r="L41" s="62" t="s">
         <v>3138</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="61" t="s">
+      <c r="M41" s="62"/>
+      <c r="N41" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O41" s="62">
+        <v>1</v>
+      </c>
+      <c r="P41" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="69" t="s">
         <v>269</v>
       </c>
-      <c r="B42" s="72" t="s">
+      <c r="B42" s="62" t="s">
         <v>3162</v>
       </c>
-      <c r="C42" s="76" t="s">
+      <c r="C42" s="75" t="s">
         <v>271</v>
       </c>
-      <c r="D42" s="73" t="s">
+      <c r="D42" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="74">
+      <c r="E42" s="71">
         <v>36164</v>
       </c>
-      <c r="F42" s="72" t="s">
+      <c r="F42" s="62" t="s">
         <v>3166</v>
       </c>
-      <c r="G42" s="65"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="73" t="s">
+      <c r="G42" s="72"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L42" s="72"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="61" t="s">
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O42" s="62">
+        <v>1</v>
+      </c>
+      <c r="P42" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="69" t="s">
         <v>272</v>
       </c>
-      <c r="B43" s="72" t="s">
+      <c r="B43" s="62" t="s">
         <v>273</v>
       </c>
-      <c r="C43" s="76" t="s">
+      <c r="C43" s="75" t="s">
         <v>274</v>
       </c>
-      <c r="D43" s="73" t="s">
+      <c r="D43" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="74">
+      <c r="E43" s="71">
         <v>36185</v>
       </c>
-      <c r="F43" s="72" t="s">
+      <c r="F43" s="62" t="s">
         <v>3166</v>
       </c>
-      <c r="G43" s="65"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="73" t="s">
+      <c r="G43" s="72"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="72" t="s">
+      <c r="L43" s="62" t="s">
         <v>3139</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="61" t="s">
+      <c r="M43" s="62"/>
+      <c r="N43" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O43" s="62">
+        <v>1</v>
+      </c>
+      <c r="P43" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="69" t="s">
         <v>3140</v>
       </c>
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="62" t="s">
         <v>3144</v>
       </c>
-      <c r="C44" s="76" t="s">
+      <c r="C44" s="75" t="s">
         <v>3141</v>
       </c>
-      <c r="D44" s="73" t="s">
+      <c r="D44" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="74">
+      <c r="E44" s="71">
         <v>38761</v>
       </c>
-      <c r="F44" s="72" t="s">
+      <c r="F44" s="62" t="s">
         <v>3167</v>
       </c>
-      <c r="G44" s="65">
+      <c r="G44" s="72">
         <v>2000</v>
       </c>
-      <c r="H44" s="72" t="s">
+      <c r="H44" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="72"/>
-      <c r="J44" s="65">
+      <c r="I44" s="62"/>
+      <c r="J44" s="72">
         <v>2000</v>
       </c>
-      <c r="K44" s="73" t="s">
+      <c r="K44" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="72" t="s">
+      <c r="L44" s="62" t="s">
         <v>3146</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="61" t="s">
+      <c r="M44" s="62">
+        <v>20</v>
+      </c>
+      <c r="N44" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O44" s="62">
+        <v>1.06</v>
+      </c>
+      <c r="P44" s="62">
+        <v>21.083333</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="69" t="s">
         <v>3142</v>
       </c>
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="62" t="s">
         <v>3145</v>
       </c>
-      <c r="C45" s="76" t="s">
+      <c r="C45" s="75" t="s">
         <v>3143</v>
       </c>
-      <c r="D45" s="73" t="s">
+      <c r="D45" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="74">
+      <c r="E45" s="71">
         <v>40347</v>
       </c>
-      <c r="F45" s="72" t="s">
+      <c r="F45" s="62" t="s">
         <v>3167</v>
       </c>
-      <c r="G45" s="65">
+      <c r="G45" s="72">
         <v>20000</v>
       </c>
-      <c r="H45" s="72" t="s">
+      <c r="H45" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I45" s="72"/>
-      <c r="J45" s="65">
+      <c r="I45" s="62"/>
+      <c r="J45" s="72">
         <v>20000</v>
       </c>
-      <c r="K45" s="73" t="s">
+      <c r="K45" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L45" s="72" t="s">
+      <c r="L45" s="62" t="s">
         <v>3147</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="61" t="s">
+      <c r="M45" s="62">
+        <v>20</v>
+      </c>
+      <c r="N45" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O45" s="62">
+        <v>1.06</v>
+      </c>
+      <c r="P45" s="62">
+        <v>21.083333</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="69" t="s">
         <v>3148</v>
       </c>
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="62" t="s">
         <v>3149</v>
       </c>
-      <c r="C46" s="76" t="s">
+      <c r="C46" s="75" t="s">
         <v>3150</v>
       </c>
-      <c r="D46" s="73" t="s">
+      <c r="D46" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="74">
+      <c r="E46" s="71">
         <v>39213</v>
       </c>
-      <c r="F46" s="72" t="s">
+      <c r="F46" s="62" t="s">
         <v>3169</v>
       </c>
-      <c r="G46" s="65">
+      <c r="G46" s="72">
         <v>1000</v>
       </c>
-      <c r="H46" s="72" t="s">
+      <c r="H46" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I46" s="72"/>
-      <c r="J46" s="72">
+      <c r="I46" s="62"/>
+      <c r="J46" s="62">
         <v>1000</v>
       </c>
-      <c r="K46" s="73" t="s">
+      <c r="K46" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L46" s="72"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="61" t="s">
+      <c r="L46" s="62"/>
+      <c r="M46" s="62"/>
+      <c r="N46" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O46" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P46" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="69" t="s">
         <v>3151</v>
       </c>
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="62" t="s">
         <v>3152</v>
       </c>
-      <c r="C47" s="76" t="s">
+      <c r="C47" s="75" t="s">
         <v>3158</v>
       </c>
-      <c r="D47" s="73" t="s">
+      <c r="D47" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E47" s="74">
+      <c r="E47" s="71">
         <v>39213</v>
       </c>
-      <c r="F47" s="72" t="s">
+      <c r="F47" s="62" t="s">
         <v>3169</v>
       </c>
-      <c r="G47" s="65"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="73" t="s">
+      <c r="G47" s="72"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L47" s="72"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="61" t="s">
+      <c r="L47" s="62"/>
+      <c r="M47" s="62"/>
+      <c r="N47" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O47" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P47" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="69" t="s">
         <v>3153</v>
       </c>
-      <c r="B48" s="72" t="s">
+      <c r="B48" s="62" t="s">
         <v>3154</v>
       </c>
-      <c r="C48" s="76" t="s">
+      <c r="C48" s="75" t="s">
         <v>3155</v>
       </c>
-      <c r="D48" s="73" t="s">
+      <c r="D48" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E48" s="74">
+      <c r="E48" s="71">
         <v>39213</v>
       </c>
-      <c r="F48" s="72" t="s">
+      <c r="F48" s="62" t="s">
         <v>3169</v>
       </c>
-      <c r="G48" s="65"/>
-      <c r="H48" s="72"/>
-      <c r="I48" s="72"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="73" t="s">
+      <c r="G48" s="72"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="L48" s="72"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="61" t="s">
+      <c r="L48" s="62"/>
+      <c r="M48" s="62"/>
+      <c r="N48" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O48" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="P48" s="62">
+        <v>17.583333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="69" t="s">
         <v>3159</v>
       </c>
-      <c r="B49" s="72" t="s">
+      <c r="B49" s="62" t="s">
         <v>3156</v>
       </c>
-      <c r="C49" s="76" t="s">
+      <c r="C49" s="75" t="s">
         <v>3157</v>
       </c>
-      <c r="D49" s="73" t="s">
+      <c r="D49" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="E49" s="74">
+      <c r="E49" s="71">
         <v>43588</v>
       </c>
-      <c r="F49" s="72" t="s">
+      <c r="F49" s="62" t="s">
         <v>3165</v>
       </c>
-      <c r="G49" s="65"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="72"/>
-      <c r="K49" s="73" t="s">
+      <c r="G49" s="72"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
+      <c r="K49" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L49" s="72"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="61" t="s">
+      <c r="L49" s="62"/>
+      <c r="M49" s="62"/>
+      <c r="N49" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O49" s="62">
+        <v>1</v>
+      </c>
+      <c r="P49" s="62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="70" t="s">
         <v>168</v>
       </c>
-      <c r="D50" s="72" t="s">
+      <c r="D50" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E50" s="74">
+      <c r="E50" s="71">
         <v>36146</v>
       </c>
-      <c r="F50" s="72"/>
-      <c r="G50" s="65">
+      <c r="F50" s="62"/>
+      <c r="G50" s="72">
         <v>10</v>
       </c>
-      <c r="H50" s="72" t="s">
+      <c r="H50" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="I50" s="72"/>
-      <c r="J50" s="72" t="s">
+      <c r="I50" s="62"/>
+      <c r="J50" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="K50" s="73" t="s">
+      <c r="K50" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L50" s="72" t="s">
+      <c r="L50" s="62" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="61" t="s">
+      <c r="M50" s="62"/>
+      <c r="N50" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O50" s="62">
+        <v>1</v>
+      </c>
+      <c r="P50" s="62">
+        <v>20.83333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="69" t="s">
         <v>180</v>
       </c>
-      <c r="B51" s="78" t="s">
+      <c r="B51" s="76" t="s">
         <v>181</v>
       </c>
-      <c r="C51" s="72" t="s">
+      <c r="C51" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="D51" s="78" t="s">
+      <c r="D51" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="E51" s="74">
+      <c r="E51" s="71">
         <v>36146</v>
       </c>
-      <c r="F51" s="72"/>
-      <c r="G51" s="65">
+      <c r="F51" s="62"/>
+      <c r="G51" s="72">
         <v>1</v>
       </c>
-      <c r="H51" s="72" t="s">
+      <c r="H51" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72" t="s">
+      <c r="I51" s="62"/>
+      <c r="J51" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="K51" s="73" t="s">
+      <c r="K51" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L51" s="72" t="s">
+      <c r="L51" s="62" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="61" t="s">
+      <c r="M51" s="62"/>
+      <c r="N51" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O51" s="62">
+        <v>1</v>
+      </c>
+      <c r="P51" s="62">
+        <v>20.83333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="B52" s="72" t="s">
+      <c r="B52" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="C52" s="73" t="s">
+      <c r="C52" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="D52" s="72" t="s">
+      <c r="D52" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E52" s="74">
+      <c r="E52" s="71">
         <v>34702</v>
       </c>
-      <c r="F52" s="72"/>
-      <c r="G52" s="65">
+      <c r="F52" s="62"/>
+      <c r="G52" s="72">
         <v>25</v>
       </c>
-      <c r="H52" s="72" t="s">
+      <c r="H52" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="I52" s="72"/>
-      <c r="J52" s="72" t="s">
+      <c r="I52" s="62"/>
+      <c r="J52" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="K52" s="73" t="s">
+      <c r="K52" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L52" s="72" t="s">
+      <c r="L52" s="62" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="61" t="s">
+      <c r="M52" s="62"/>
+      <c r="N52" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O52" s="62">
+        <v>1</v>
+      </c>
+      <c r="P52" s="62">
+        <v>20.83333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="B53" s="72" t="s">
+      <c r="B53" s="62" t="s">
         <v>219</v>
       </c>
-      <c r="C53" s="73" t="s">
+      <c r="C53" s="70" t="s">
         <v>220</v>
       </c>
-      <c r="D53" s="72" t="s">
+      <c r="D53" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E53" s="74">
+      <c r="E53" s="71">
         <v>34702</v>
       </c>
-      <c r="F53" s="72"/>
-      <c r="G53" s="65">
+      <c r="F53" s="62"/>
+      <c r="G53" s="72">
         <v>5</v>
       </c>
-      <c r="H53" s="72" t="s">
+      <c r="H53" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="I53" s="72"/>
-      <c r="J53" s="72" t="s">
+      <c r="I53" s="62"/>
+      <c r="J53" s="62" t="s">
         <v>221</v>
       </c>
-      <c r="K53" s="73" t="s">
+      <c r="K53" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L53" s="72" t="s">
+      <c r="L53" s="62" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="62"/>
+      <c r="N53" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O53" s="62">
+        <v>1</v>
+      </c>
+      <c r="P53" s="62">
+        <v>20.83333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="77" t="s">
         <v>227</v>
       </c>
-      <c r="B54" s="72" t="s">
+      <c r="B54" s="62" t="s">
         <v>228</v>
       </c>
-      <c r="C54" s="76" t="s">
+      <c r="C54" s="75" t="s">
         <v>229</v>
       </c>
-      <c r="D54" s="72" t="s">
+      <c r="D54" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E54" s="74">
+      <c r="E54" s="71">
         <v>35132</v>
       </c>
-      <c r="F54" s="72"/>
-      <c r="G54" s="65"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
-      <c r="K54" s="73" t="s">
+      <c r="F54" s="62"/>
+      <c r="G54" s="72"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="62"/>
+      <c r="K54" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L54" s="72" t="s">
+      <c r="L54" s="62" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="62"/>
+      <c r="N54" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O54" s="62">
+        <v>1</v>
+      </c>
+      <c r="P54" s="62">
+        <v>20.83333</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="77" t="s">
         <v>231</v>
       </c>
-      <c r="B55" s="72" t="s">
+      <c r="B55" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="C55" s="76" t="s">
+      <c r="C55" s="75" t="s">
         <v>233</v>
       </c>
-      <c r="D55" s="72" t="s">
+      <c r="D55" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E55" s="74">
+      <c r="E55" s="71">
         <v>38147</v>
       </c>
-      <c r="F55" s="72"/>
-      <c r="G55" s="65"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="72"/>
-      <c r="J55" s="72"/>
-      <c r="K55" s="73" t="s">
+      <c r="F55" s="62"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="62"/>
+      <c r="I55" s="62"/>
+      <c r="J55" s="62"/>
+      <c r="K55" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L55" s="72" t="s">
+      <c r="L55" s="62" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="61" t="s">
+      <c r="M55" s="62"/>
+      <c r="N55" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O55" s="62">
+        <v>1</v>
+      </c>
+      <c r="P55" s="62">
+        <v>20.83333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="69" t="s">
         <v>235</v>
       </c>
-      <c r="B56" s="72" t="s">
+      <c r="B56" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="C56" s="73" t="s">
+      <c r="C56" s="70" t="s">
         <v>237</v>
       </c>
-      <c r="D56" s="72" t="s">
+      <c r="D56" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E56" s="74">
+      <c r="E56" s="71">
         <v>35530</v>
       </c>
-      <c r="F56" s="72"/>
-      <c r="G56" s="65"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="72"/>
-      <c r="K56" s="73" t="s">
+      <c r="F56" s="62"/>
+      <c r="G56" s="72"/>
+      <c r="H56" s="62"/>
+      <c r="I56" s="62"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L56" s="72" t="s">
+      <c r="L56" s="62" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="61" t="s">
+      <c r="M56" s="62"/>
+      <c r="N56" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O56" s="62">
+        <v>1</v>
+      </c>
+      <c r="P56" s="62">
+        <v>20.83333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="69" t="s">
         <v>253</v>
       </c>
-      <c r="B57" s="72" t="s">
+      <c r="B57" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="C57" s="72" t="s">
+      <c r="C57" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="D57" s="73" t="s">
+      <c r="D57" s="70" t="s">
         <v>256</v>
       </c>
-      <c r="E57" s="74">
+      <c r="E57" s="71">
         <v>38187</v>
       </c>
-      <c r="F57" s="72"/>
-      <c r="G57" s="65">
+      <c r="F57" s="62"/>
+      <c r="G57" s="72">
         <v>50</v>
       </c>
-      <c r="H57" s="72" t="s">
+      <c r="H57" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I57" s="73"/>
-      <c r="J57" s="65">
+      <c r="I57" s="70"/>
+      <c r="J57" s="72">
         <v>50</v>
       </c>
-      <c r="K57" s="73" t="s">
+      <c r="K57" s="70" t="s">
         <v>3133</v>
       </c>
-      <c r="L57" s="72" t="s">
+      <c r="L57" s="62" t="s">
         <v>3134</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="61" t="s">
+      <c r="M57" s="62"/>
+      <c r="N57" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O57" s="62">
+        <v>1</v>
+      </c>
+      <c r="P57" s="62">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="C58" s="76" t="s">
+      <c r="C58" s="75" t="s">
         <v>262</v>
       </c>
-      <c r="D58" s="73" t="s">
+      <c r="D58" s="70" t="s">
         <v>256</v>
       </c>
-      <c r="E58" s="74">
+      <c r="E58" s="71">
         <v>37834</v>
       </c>
-      <c r="F58" s="72"/>
-      <c r="G58" s="65">
+      <c r="F58" s="62"/>
+      <c r="G58" s="72">
         <v>150</v>
       </c>
-      <c r="H58" s="72" t="s">
+      <c r="H58" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I58" s="72"/>
-      <c r="J58" s="65">
+      <c r="I58" s="62"/>
+      <c r="J58" s="72">
         <v>150</v>
       </c>
-      <c r="K58" s="73" t="s">
+      <c r="K58" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="L58" s="72" t="s">
+      <c r="L58" s="62" t="s">
         <v>3136</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="61" t="s">
+      <c r="M58" s="62">
+        <v>7.5</v>
+      </c>
+      <c r="N58" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O58" s="62">
+        <v>1</v>
+      </c>
+      <c r="P58" s="62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="69" t="s">
         <v>134</v>
       </c>
-      <c r="B59" s="72" t="s">
+      <c r="B59" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="73" t="s">
+      <c r="C59" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="72" t="s">
+      <c r="D59" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="E59" s="74">
+      <c r="E59" s="71">
         <v>38687</v>
       </c>
-      <c r="F59" s="72"/>
-      <c r="G59" s="65">
+      <c r="F59" s="62"/>
+      <c r="G59" s="72">
         <v>10</v>
       </c>
-      <c r="H59" s="72" t="s">
+      <c r="H59" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I59" s="72"/>
-      <c r="J59" s="72">
+      <c r="I59" s="62"/>
+      <c r="J59" s="62">
         <v>10</v>
       </c>
-      <c r="K59" s="73" t="s">
+      <c r="K59" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="L59" s="72" t="s">
+      <c r="L59" s="62" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="61" t="s">
+      <c r="M59" s="62">
+        <v>10</v>
+      </c>
+      <c r="N59" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O59" s="62">
+        <v>1</v>
+      </c>
+      <c r="P59" s="62">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="72" t="s">
+      <c r="B60" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="C60" s="73" t="s">
+      <c r="C60" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="D60" s="72" t="s">
+      <c r="D60" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="E60" s="74">
+      <c r="E60" s="71">
         <v>34702</v>
       </c>
-      <c r="F60" s="72"/>
-      <c r="G60" s="65">
+      <c r="F60" s="62"/>
+      <c r="G60" s="72">
         <v>10</v>
       </c>
-      <c r="H60" s="72" t="s">
+      <c r="H60" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="I60" s="72"/>
-      <c r="J60" s="72" t="s">
+      <c r="I60" s="62"/>
+      <c r="J60" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="K60" s="73" t="s">
+      <c r="K60" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L60" s="72" t="s">
+      <c r="L60" s="62" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="61" t="s">
+      <c r="N60" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O60" s="62">
+        <v>1</v>
+      </c>
+      <c r="P60" s="62">
+        <v>7.4166660000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="72" t="s">
+      <c r="B61" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="C61" s="73" t="s">
+      <c r="C61" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="78" t="s">
+      <c r="D61" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="E61" s="74">
+      <c r="E61" s="71">
         <v>40805</v>
       </c>
-      <c r="F61" s="72"/>
-      <c r="G61" s="65">
+      <c r="F61" s="62"/>
+      <c r="G61" s="72">
         <v>100</v>
       </c>
-      <c r="H61" s="72" t="s">
+      <c r="H61" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I61" s="72"/>
-      <c r="J61" s="72">
+      <c r="I61" s="62"/>
+      <c r="J61" s="62">
         <v>100</v>
       </c>
-      <c r="K61" s="73" t="s">
+      <c r="K61" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L61" s="72" t="s">
+      <c r="L61" s="62" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="61" t="s">
+      <c r="M61" s="62">
+        <v>0.25</v>
+      </c>
+      <c r="N61" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O61" s="62">
+        <v>1</v>
+      </c>
+      <c r="P61" s="62">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="B62" s="72" t="s">
+      <c r="B62" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="70" t="s">
         <v>128</v>
       </c>
-      <c r="D62" s="72" t="s">
+      <c r="D62" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E62" s="74">
+      <c r="E62" s="71">
         <v>34702</v>
       </c>
-      <c r="F62" s="72"/>
-      <c r="G62" s="65">
+      <c r="F62" s="62"/>
+      <c r="G62" s="72">
         <v>1000</v>
       </c>
-      <c r="H62" s="72" t="s">
+      <c r="H62" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72">
+      <c r="I62" s="62"/>
+      <c r="J62" s="62">
         <v>1000</v>
       </c>
-      <c r="K62" s="73" t="s">
+      <c r="K62" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L62" s="72" t="s">
+      <c r="L62" s="62" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="61" t="s">
+      <c r="M62" s="62">
+        <v>0.01</v>
+      </c>
+      <c r="N62" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O62" s="62">
+        <v>1</v>
+      </c>
+      <c r="P62" s="62">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="B63" s="72" t="s">
+      <c r="B63" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="C63" s="73" t="s">
+      <c r="C63" s="70" t="s">
         <v>147</v>
       </c>
-      <c r="D63" s="72" t="s">
+      <c r="D63" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="E63" s="74">
+      <c r="E63" s="71">
         <v>43252</v>
       </c>
-      <c r="F63" s="72"/>
-      <c r="G63" s="65">
+      <c r="F63" s="62"/>
+      <c r="G63" s="72">
         <v>2500</v>
       </c>
-      <c r="H63" s="72" t="s">
+      <c r="H63" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="I63" s="72"/>
-      <c r="J63" s="72" t="s">
+      <c r="I63" s="62"/>
+      <c r="J63" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="K63" s="73" t="s">
+      <c r="K63" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L63" s="72" t="s">
+      <c r="L63" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="61" t="s">
+      <c r="M63" s="62"/>
+      <c r="N63" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O63" s="62">
+        <v>1</v>
+      </c>
+      <c r="P63" s="62">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="69" t="s">
         <v>151</v>
       </c>
-      <c r="B64" s="72" t="s">
+      <c r="B64" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="C64" s="73" t="s">
+      <c r="C64" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="D64" s="72" t="s">
+      <c r="D64" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="E64" s="74">
+      <c r="E64" s="71">
         <v>37631</v>
       </c>
-      <c r="F64" s="72"/>
-      <c r="G64" s="65">
+      <c r="F64" s="62"/>
+      <c r="G64" s="72">
         <v>2500</v>
       </c>
-      <c r="H64" s="72" t="s">
+      <c r="H64" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="I64" s="72"/>
-      <c r="J64" s="72" t="s">
+      <c r="I64" s="62"/>
+      <c r="J64" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="K64" s="73" t="s">
+      <c r="K64" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L64" s="72" t="s">
+      <c r="L64" s="62" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="61" t="s">
+      <c r="M64" s="62"/>
+      <c r="N64" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O64" s="62">
+        <v>1</v>
+      </c>
+      <c r="P64" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="69" t="s">
         <v>176</v>
       </c>
-      <c r="B65" s="72" t="s">
+      <c r="B65" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="C65" s="73" t="s">
+      <c r="C65" s="70" t="s">
         <v>178</v>
       </c>
-      <c r="D65" s="72" t="s">
+      <c r="D65" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="E65" s="74">
+      <c r="E65" s="71">
         <v>35240</v>
       </c>
-      <c r="F65" s="72"/>
-      <c r="G65" s="65">
+      <c r="F65" s="62"/>
+      <c r="G65" s="72">
         <v>10</v>
       </c>
-      <c r="H65" s="72" t="s">
+      <c r="H65" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="I65" s="72"/>
-      <c r="J65" s="72" t="s">
+      <c r="I65" s="62"/>
+      <c r="J65" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="K65" s="73" t="s">
+      <c r="K65" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="L65" s="72" t="s">
+      <c r="L65" s="62" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="61" t="s">
+      <c r="M65" s="62"/>
+      <c r="N65" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O65" s="62">
+        <v>1</v>
+      </c>
+      <c r="P65" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="72" t="s">
+      <c r="B66" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="C66" s="75" t="s">
+      <c r="C66" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="D66" s="72" t="s">
+      <c r="D66" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="E66" s="74">
+      <c r="E66" s="71">
         <v>34702</v>
       </c>
-      <c r="F66" s="72"/>
-      <c r="G66" s="65">
+      <c r="F66" s="62"/>
+      <c r="G66" s="72">
         <v>500</v>
       </c>
-      <c r="H66" s="72" t="s">
+      <c r="H66" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I66" s="72"/>
-      <c r="J66" s="72">
+      <c r="I66" s="62"/>
+      <c r="J66" s="62">
         <v>500</v>
       </c>
-      <c r="K66" s="73" t="s">
+      <c r="K66" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="L66" s="72" t="s">
+      <c r="L66" s="62" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="61" t="s">
+      <c r="M66" s="62">
+        <v>5</v>
+      </c>
+      <c r="N66" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O66" s="62">
+        <v>1</v>
+      </c>
+      <c r="P66" s="62">
+        <v>17.33333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="75" t="s">
+      <c r="C67" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="D67" s="72" t="s">
+      <c r="D67" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="E67" s="74">
+      <c r="E67" s="71">
         <v>34708</v>
       </c>
-      <c r="F67" s="72"/>
-      <c r="G67" s="65">
+      <c r="F67" s="62"/>
+      <c r="G67" s="72">
         <v>375</v>
       </c>
-      <c r="H67" s="72" t="s">
+      <c r="H67" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I67" s="72"/>
-      <c r="J67" s="72">
+      <c r="I67" s="62"/>
+      <c r="J67" s="62">
         <v>375</v>
       </c>
-      <c r="K67" s="73" t="s">
+      <c r="K67" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="L67" s="72" t="s">
+      <c r="L67" s="62" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="61" t="s">
+      <c r="M67" s="62">
+        <v>18.75</v>
+      </c>
+      <c r="N67" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O67" s="62">
+        <v>1</v>
+      </c>
+      <c r="P67" s="62">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="C68" s="75" t="s">
+      <c r="C68" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="D68" s="72" t="s">
+      <c r="D68" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="E68" s="74">
+      <c r="E68" s="71">
         <v>34702</v>
       </c>
-      <c r="F68" s="72"/>
-      <c r="G68" s="65">
+      <c r="F68" s="62"/>
+      <c r="G68" s="72">
         <v>10</v>
       </c>
-      <c r="H68" s="72" t="s">
+      <c r="H68" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I68" s="72"/>
-      <c r="J68" s="72">
+      <c r="I68" s="62"/>
+      <c r="J68" s="62">
         <v>10</v>
       </c>
-      <c r="K68" s="73" t="s">
+      <c r="K68" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L68" s="72" t="s">
+      <c r="L68" s="62" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="61" t="s">
+      <c r="M68" s="62">
+        <v>10</v>
+      </c>
+      <c r="N68" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O68" s="62">
+        <v>1</v>
+      </c>
+      <c r="P68" s="62">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="B69" s="72" t="s">
+      <c r="B69" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="C69" s="73" t="s">
+      <c r="C69" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="D69" s="72" t="s">
+      <c r="D69" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="E69" s="74">
+      <c r="E69" s="71">
         <v>34702</v>
       </c>
-      <c r="F69" s="72"/>
-      <c r="G69" s="65">
+      <c r="F69" s="62"/>
+      <c r="G69" s="72">
         <v>112</v>
       </c>
-      <c r="H69" s="72" t="s">
+      <c r="H69" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I69" s="72"/>
-      <c r="J69" s="72">
+      <c r="I69" s="62"/>
+      <c r="J69" s="62">
         <v>112</v>
       </c>
-      <c r="K69" s="73" t="s">
+      <c r="K69" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="L69" s="72" t="s">
+      <c r="L69" s="62" t="s">
         <v>161</v>
+      </c>
+      <c r="M69" s="62">
+        <v>11.2</v>
+      </c>
+      <c r="N69" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="O69" s="62">
+        <v>1</v>
+      </c>
+      <c r="P69" s="62">
+        <v>9.5</v>
       </c>
     </row>
   </sheetData>
@@ -13114,13 +13930,13 @@
     <sortCondition ref="D3:D69"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0043C0CD-5EB1-4F0C-BB33-C75AF9D10A28}">
           <x14:formula1>
             <xm:f>'Custom-Anurag'!$A$2:$A$11</xm:f>
@@ -13144,7 +13960,7 @@
   <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B23" sqref="B23:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15638,11 +16454,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="49" t="s">
         <v>477</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -16163,10 +16979,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="49" t="s">
         <v>565</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="49"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">

</xml_diff>